<commit_message>
draft restful API framework finished.
</commit_message>
<xml_diff>
--- a/api/testData/api_test_cases_multi_flow.xlsx
+++ b/api/testData/api_test_cases_multi_flow.xlsx
@@ -1,19 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cowry\Desktop\fastapi\autotestgit\api\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cowry\Desktop\fastapi\autotestgit\api\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EC93F391-A17F-4E47-801F-61E41CA5E697}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A699B897-E2AA-4382-BA0A-5698208C3A58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="690" windowWidth="21570" windowHeight="11745" xr2:uid="{EFBB3CF1-3761-4F64-9C29-7999EAF6939F}"/>
+    <workbookView xWindow="1065" yWindow="2025" windowWidth="21510" windowHeight="10005" activeTab="2" xr2:uid="{EFBB3CF1-3761-4F64-9C29-7999EAF6939F}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="pre_process" sheetId="7" r:id="rId1"/>
+    <sheet name="after_process" sheetId="8" r:id="rId2"/>
+    <sheet name="users" sheetId="1" r:id="rId3"/>
+    <sheet name="products" sheetId="2" r:id="rId4"/>
+    <sheet name="orders" sheetId="3" r:id="rId5"/>
+    <sheet name="payments" sheetId="4" r:id="rId6"/>
+    <sheet name="shipments" sheetId="5" r:id="rId7"/>
+    <sheet name="Sheet6" sheetId="6" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,27 +43,78 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
-  <si>
-    <t>user</t>
-  </si>
-  <si>
-    <t>passwd</t>
-  </si>
-  <si>
-    <t>result</t>
-  </si>
-  <si>
-    <t>abc</t>
-  </si>
-  <si>
-    <t>{"code": 0, "msg": "Login ok"}</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>{"code": 1, "msg": "username or password error"}</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+  <si>
+    <t>case_id</t>
+  </si>
+  <si>
+    <t>interface</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>method</t>
+  </si>
+  <si>
+    <t>url</t>
+  </si>
+  <si>
+    <t>request_data</t>
+  </si>
+  <si>
+    <t>expected</t>
+  </si>
+  <si>
+    <t>user added successfully</t>
+  </si>
+  <si>
+    <t>post</t>
+  </si>
+  <si>
+    <t>/paymall_admin/users/</t>
+  </si>
+  <si>
+    <t>{"username":"#username#","mobile":"#phone#","password":"#password#","email":"a@a.com"}</t>
+  </si>
+  <si>
+    <t>{"id":#id#,"username":"#username#","mobile":"#phone#","email":"a@a.com"}</t>
+  </si>
+  <si>
+    <t>login pass, username, password</t>
+  </si>
+  <si>
+    <t>/paymall_admin/authorizations/</t>
+  </si>
+  <si>
+    <t>{"refresh":"#refresh_token#", "access":"#access_token#"}</t>
+  </si>
+  <si>
+    <t>login</t>
+  </si>
+  <si>
+    <t>{"username": "#username#", "password": "#password#"}</t>
+  </si>
+  <si>
+    <t>users_list</t>
+  </si>
+  <si>
+    <t>users_add</t>
+  </si>
+  <si>
+    <t>list current users</t>
+  </si>
+  <si>
+    <t>get</t>
+  </si>
+  <si>
+    <t>extract_data</t>
+  </si>
+  <si>
+    <t>/paymall_admin/statistical/total_count/</t>
+  </si>
+  <si>
+    <t>{"count":#count#}</t>
   </si>
 </sst>
 </file>
@@ -408,21 +466,53 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E18549D-56CB-404D-B9B3-142CDF6C6474}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8010984-AFC9-4623-8CFF-B57F08B9E56D}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA226EC8-69BF-4338-AEC9-E24BC31576C9}">
-  <dimension ref="A1:C4"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+  <dimension ref="A1:H4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" customWidth="1"/>
-    <col min="3" max="3" width="48.85546875" customWidth="1"/>
+    <col min="1" max="1" width="8.5703125" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" customWidth="1"/>
+    <col min="3" max="3" width="30.28515625" customWidth="1"/>
+    <col min="5" max="5" width="37.140625" customWidth="1"/>
+    <col min="6" max="6" width="86.28515625" customWidth="1"/>
+    <col min="7" max="7" width="58.85546875" customWidth="1"/>
+    <col min="8" max="8" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -432,41 +522,153 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:8">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AEDB628-90C3-45E3-91A3-710C9E179EB9}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E64F61B-9C9D-4C2C-A51B-813C9D70078E}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0A5E8B2-1A1A-4A9B-8A2E-B848F4A52E31}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA748851-EA21-4671-AA5B-3350AAE052C5}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C6B08A5-7FD5-4D39-BDEC-1836E33CC778}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>